<commit_message>
Expense Sheet read and display
</commit_message>
<xml_diff>
--- a/Features to Implement.xlsx
+++ b/Features to Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Serial</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Page where you can change claims given to a paritcular user</t>
+  </si>
+  <si>
+    <t>Background Jobs</t>
+  </si>
+  <si>
+    <t>Excel sheet of montly expense to be processed by background job</t>
+  </si>
+  <si>
+    <t>Upload file control</t>
+  </si>
+  <si>
+    <t>Backend Apis</t>
+  </si>
+  <si>
+    <t>Api Controllers need to be moved to a separate project</t>
   </si>
 </sst>
 </file>
@@ -405,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -416,7 +431,7 @@
     <col min="1" max="1" width="5.06640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -512,14 +527,37 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expense Sheet -- in Progress
... webpack failure
</commit_message>
<xml_diff>
--- a/Features to Implement.xlsx
+++ b/Features to Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Serial</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>Api Controllers need to be moved to a separate project</t>
+  </si>
+  <si>
+    <t>Loggin &amp; Instrumentation</t>
+  </si>
+  <si>
+    <t>Using Serilog with .net Core projects for DI</t>
+  </si>
+  <si>
+    <t>Add Serilog Logger to Aspnet Core Web</t>
+  </si>
+  <si>
+    <t>Add Serilog Logger to Web Apis'</t>
+  </si>
+  <si>
+    <t>File Manager</t>
+  </si>
+  <si>
+    <t>Add files grouped by folders… for salary slips…. Look at UI in theme "File Manager"</t>
   </si>
 </sst>
 </file>
@@ -420,16 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.06640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.3984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -501,63 +519,89 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C21" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and Seeded Data for Mapping
</commit_message>
<xml_diff>
--- a/Features to Implement.xlsx
+++ b/Features to Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Serial</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Add files grouped by folders… for salary slips…. Look at UI in theme "File Manager"</t>
+  </si>
+  <si>
+    <t>Monthly expenses uploaded files should be tracked…and retained for later download… After one year archive them.</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -604,6 +607,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Filtering of sources added
</commit_message>
<xml_diff>
--- a/Features to Implement.xlsx
+++ b/Features to Implement.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C2BE77-AD7B-490B-9AC4-0089B652C58D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,12 +100,6 @@
     <t>Upload file control</t>
   </si>
   <si>
-    <t>Backend Apis</t>
-  </si>
-  <si>
-    <t>Api Controllers need to be moved to a separate project</t>
-  </si>
-  <si>
     <t>Loggin &amp; Instrumentation</t>
   </si>
   <si>
@@ -124,12 +119,18 @@
   </si>
   <si>
     <t>Monthly expenses uploaded files should be tracked…and retained for later download… After one year archive them.</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Toastr Integration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,11 +441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -575,41 +576,41 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AE-54: Front End service for category Mappings
</commit_message>
<xml_diff>
--- a/Features to Implement.xlsx
+++ b/Features to Implement.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FD397-842E-4A41-B51D-7064F111515A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A474A-A7A2-4D45-9B8B-0839B0816157}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Serial</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Excel Import / Export</t>
+  </si>
+  <si>
+    <t>An excel export of records</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -528,151 +534,162 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.95" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.95" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C11" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="C14" t="s">
+    <row r="17" spans="2:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C15" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
-        <v>23</v>
+      <c r="C25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C27" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C30" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C33" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C34" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B37" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
         <v>30</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C38" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -685,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400A4D46-E08A-4B46-988E-7F61479ED277}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>

</xml_diff>